<commit_message>
corregi el stem plot
</commit_message>
<xml_diff>
--- a/sedDegr.xlsx
+++ b/sedDegr.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="75">
   <si>
     <t>Sample</t>
   </si>
@@ -168,6 +168,21 @@
     <t>site</t>
   </si>
   <si>
+    <r>
+      <t>β</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>-Sitosterol</t>
+    </r>
+  </si>
+  <si>
     <t>Acc Eff</t>
   </si>
   <si>
@@ -175,6 +190,83 @@
   </si>
   <si>
     <t>V Flux</t>
+  </si>
+  <si>
+    <r>
+      <t>69</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>±108</t>
+    </r>
+  </si>
+  <si>
+    <t>3.6±4.1</t>
+  </si>
+  <si>
+    <t>9.8±14</t>
+  </si>
+  <si>
+    <t>5.8±9.4</t>
+  </si>
+  <si>
+    <t>4.2±7.5</t>
+  </si>
+  <si>
+    <t>0.40±0.36</t>
+  </si>
+  <si>
+    <t>1.3±1.6</t>
+  </si>
+  <si>
+    <t>0.42±0.57</t>
+  </si>
+  <si>
+    <t>16±26</t>
+  </si>
+  <si>
+    <t>2.0±4.3</t>
+  </si>
+  <si>
+    <t>3.2±4.6</t>
+  </si>
+  <si>
+    <t>0.60±0.83</t>
+  </si>
+  <si>
+    <t>0.71±0.98</t>
+  </si>
+  <si>
+    <t>0.96±1.1</t>
+  </si>
+  <si>
+    <t>0.72±1.7</t>
+  </si>
+  <si>
+    <t>16±28</t>
+  </si>
+  <si>
+    <t>6.7±7.5</t>
+  </si>
+  <si>
+    <t>7.0±12</t>
+  </si>
+  <si>
+    <t>7.4±11</t>
+  </si>
+  <si>
+    <t>25±57</t>
+  </si>
+  <si>
+    <t>0.52±0.79</t>
+  </si>
+  <si>
+    <t>4.7±14</t>
   </si>
 </sst>
 </file>
@@ -191,7 +283,7 @@
     <numFmt numFmtId="170" formatCode="0.00E+000"/>
     <numFmt numFmtId="171" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -235,6 +327,19 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -311,7 +416,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,6 +502,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8051,10 +8168,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
+      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8081,8 +8198,8 @@
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
+      <c r="G1" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>11</v>
@@ -8105,7 +8222,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>24</v>
@@ -8146,7 +8263,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>25</v>
@@ -8187,7 +8304,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>24</v>
@@ -8228,7 +8345,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>25</v>
@@ -8269,7 +8386,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>24</v>
@@ -8277,7 +8394,7 @@
       <c r="C6" s="0" t="n">
         <v>69.4866667310927</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="23" t="n">
         <v>3.55495857846617</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -8310,7 +8427,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>24</v>
@@ -8351,7 +8468,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>25</v>
@@ -8392,7 +8509,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>25</v>
@@ -8432,44 +8549,85 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>12</v>
+      <c r="A10" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subo grafico acceff modificado
</commit_message>
<xml_diff>
--- a/sedDegr.xlsx
+++ b/sedDegr.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="77">
   <si>
     <t>Sample</t>
   </si>
@@ -236,6 +236,9 @@
     <t>3.2±4.6</t>
   </si>
   <si>
+    <t>116±68</t>
+  </si>
+  <si>
     <t>0.60±0.83</t>
   </si>
   <si>
@@ -268,12 +271,15 @@
   <si>
     <t>4.7±14</t>
   </si>
+  <si>
+    <t>70±125</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
@@ -282,8 +288,9 @@
     <numFmt numFmtId="169" formatCode="0.0"/>
     <numFmt numFmtId="170" formatCode="0.00E+000"/>
     <numFmt numFmtId="171" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="172" formatCode="0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -334,6 +341,13 @@
       <b val="true"/>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -416,7 +430,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -509,11 +523,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3806,8 +3828,8 @@
   </sheetPr>
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3890,7 +3912,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -3955,7 +3977,8 @@
         <v>0</v>
       </c>
       <c r="V2" s="7" t="n">
-        <v>0.00186162297915148</v>
+        <f aca="false">SUM(E2:U2)</f>
+        <v>7.01859959723174E-006</v>
       </c>
       <c r="W2" s="7" t="n">
         <v>0.0014276214083062</v>
@@ -3964,7 +3987,7 @@
         <v>0.000176170854287463</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -4029,7 +4052,8 @@
         <v>0</v>
       </c>
       <c r="V3" s="7" t="n">
-        <v>0.00479788935833296</v>
+        <f aca="false">SUM(E3:U3)</f>
+        <v>2.81983929729681E-005</v>
       </c>
       <c r="W3" s="7" t="n">
         <v>0.00338807247292815</v>
@@ -4038,7 +4062,7 @@
         <v>0.000514385764894431</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -4103,7 +4127,8 @@
         <v>0</v>
       </c>
       <c r="V4" s="7" t="n">
-        <v>0.0097597072707799</v>
+        <f aca="false">SUM(E4:U4)</f>
+        <v>0.000100062970039694</v>
       </c>
       <c r="W4" s="7" t="n">
         <v>0.00673451826907287</v>
@@ -4112,7 +4137,7 @@
         <v>0.00111113507965663</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -4177,7 +4202,8 @@
         <v>0</v>
       </c>
       <c r="V5" s="7" t="n">
-        <v>0.0068639066926433</v>
+        <f aca="false">SUM(E5:U5)</f>
+        <v>5.15617950710118E-005</v>
       </c>
       <c r="W5" s="7" t="n">
         <v>0.00479275707643505</v>
@@ -4186,7 +4212,7 @@
         <v>0.000781486107830324</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -4251,7 +4277,8 @@
         <v>0</v>
       </c>
       <c r="V6" s="7" t="n">
-        <v>0.0817309862945637</v>
+        <f aca="false">SUM(E6:U6)</f>
+        <v>0.00142903980910201</v>
       </c>
       <c r="W6" s="7" t="n">
         <v>0.0623996833891793</v>
@@ -4260,7 +4287,7 @@
         <v>0.00286309216619981</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -4325,7 +4352,8 @@
         <v>0</v>
       </c>
       <c r="V7" s="7" t="n">
-        <v>0.0395041976442048</v>
+        <f aca="false">SUM(E7:U7)</f>
+        <v>0.00015195351142161</v>
       </c>
       <c r="W7" s="7" t="n">
         <v>0.0284510583724961</v>
@@ -4334,7 +4362,7 @@
         <v>0.00457669950824774</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -4399,7 +4427,8 @@
         <v>0</v>
       </c>
       <c r="V8" s="7" t="n">
-        <v>0.0118727201991908</v>
+        <f aca="false">SUM(E8:U8)</f>
+        <v>5.96378229179179E-005</v>
       </c>
       <c r="W8" s="7" t="n">
         <v>0.0118727201991908</v>
@@ -4408,7 +4437,7 @@
         <v>0.0011829474011827</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -4473,7 +4502,8 @@
         <v>0</v>
       </c>
       <c r="V9" s="7" t="n">
-        <v>0.0168079231248055</v>
+        <f aca="false">SUM(E9:U9)</f>
+        <v>0.000122268224004233</v>
       </c>
       <c r="W9" s="7" t="n">
         <v>0.0168079231248055</v>
@@ -4482,7 +4512,7 @@
         <v>0.00160342545907252</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -4547,7 +4577,8 @@
         <v>0</v>
       </c>
       <c r="V10" s="7" t="n">
-        <v>0.0155620964830377</v>
+        <f aca="false">SUM(E10:U10)</f>
+        <v>0.000153919031680761</v>
       </c>
       <c r="W10" s="7" t="n">
         <v>0</v>
@@ -4556,7 +4587,7 @@
         <v>0.00106083753501401</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -4621,7 +4652,8 @@
         <v>0</v>
       </c>
       <c r="V11" s="7" t="n">
-        <v>0.0753801353999191</v>
+        <f aca="false">SUM(E11:U11)</f>
+        <v>0.00114146833051502</v>
       </c>
       <c r="W11" s="7" t="n">
         <v>0.0613316337005727</v>
@@ -4630,7 +4662,7 @@
         <v>0.0024162936756925</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -4695,7 +4727,8 @@
         <v>0</v>
       </c>
       <c r="V12" s="7" t="n">
-        <v>0.0110372807625874</v>
+        <f aca="false">SUM(E12:U12)</f>
+        <v>4.56392027574174E-005</v>
       </c>
       <c r="W12" s="7" t="n">
         <v>0.00808909050606186</v>
@@ -4704,7 +4737,7 @@
         <v>0.00108791700528768</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -4769,7 +4802,8 @@
         <v>0</v>
       </c>
       <c r="V13" s="7" t="n">
-        <v>0.041529698286526</v>
+        <f aca="false">SUM(E13:U13)</f>
+        <v>0.000562512528487591</v>
       </c>
       <c r="W13" s="7" t="n">
         <v>0.0342047614455674</v>
@@ -4778,7 +4812,7 @@
         <v>0.00126615714752568</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -4843,7 +4877,8 @@
         <v>0</v>
       </c>
       <c r="V14" s="7" t="n">
-        <v>0.00481898476349576</v>
+        <f aca="false">SUM(E14:U14)</f>
+        <v>5.04705284311925E-005</v>
       </c>
       <c r="W14" s="7" t="n">
         <v>0.00313070637584664</v>
@@ -4852,7 +4887,7 @@
         <v>0.00072651601301265</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
@@ -4917,7 +4952,8 @@
         <v>0</v>
       </c>
       <c r="V15" s="7" t="n">
-        <v>0.00340948127538477</v>
+        <f aca="false">SUM(E15:U15)</f>
+        <v>1.796510464276E-005</v>
       </c>
       <c r="W15" s="7" t="n">
         <v>0.00243344254968238</v>
@@ -4926,7 +4962,7 @@
         <v>0.000400818299282602</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -4991,7 +5027,8 @@
         <v>0</v>
       </c>
       <c r="V16" s="7" t="n">
-        <v>0.00493838970774339</v>
+        <f aca="false">SUM(E16:U16)</f>
+        <v>6.18753504491642E-005</v>
       </c>
       <c r="W16" s="7" t="n">
         <v>0.00421680282934813</v>
@@ -5000,7 +5037,7 @@
         <v>0.000236901720923407</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
@@ -5065,7 +5102,8 @@
         <v>0</v>
       </c>
       <c r="V17" s="7" t="n">
-        <v>0.0355748589432285</v>
+        <f aca="false">SUM(E17:U17)</f>
+        <v>0.0011425071113728</v>
       </c>
       <c r="W17" s="7" t="n">
         <v>0.0241190679893542</v>
@@ -5074,7 +5112,7 @@
         <v>0.003440045234134</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -5139,7 +5177,8 @@
         <v>0</v>
       </c>
       <c r="V18" s="7" t="n">
-        <v>0.0123647599151417</v>
+        <f aca="false">SUM(E18:U18)</f>
+        <v>0.000287360824956114</v>
       </c>
       <c r="W18" s="7" t="n">
         <v>0.0103696151760344</v>
@@ -5148,7 +5187,7 @@
         <v>0.000420417000219476</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
@@ -5213,7 +5252,8 @@
         <v>1.70542216982774E-011</v>
       </c>
       <c r="V19" s="7" t="n">
-        <v>1.13367402116402E-005</v>
+        <f aca="false">SUM(E19:U19)</f>
+        <v>4.14132739698699E-009</v>
       </c>
       <c r="W19" s="7" t="n">
         <v>4.3160171179583E-007</v>
@@ -5222,7 +5262,7 @@
         <v>7.74478680361033E-006</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
         <v>25</v>
       </c>
@@ -5287,7 +5327,8 @@
         <v>0</v>
       </c>
       <c r="V20" s="7" t="n">
-        <v>3.31036290071584E-006</v>
+        <f aca="false">SUM(E20:U20)</f>
+        <v>1.16889045730205E-009</v>
       </c>
       <c r="W20" s="7" t="n">
         <v>1.22236539060068E-007</v>
@@ -5296,7 +5337,7 @@
         <v>2.11574852163087E-006</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
         <v>25</v>
       </c>
@@ -5361,7 +5402,8 @@
         <v>0</v>
       </c>
       <c r="V21" s="7" t="n">
-        <v>1.29560209772798E-005</v>
+        <f aca="false">SUM(E21:U21)</f>
+        <v>6.5989512360688E-010</v>
       </c>
       <c r="W21" s="7" t="n">
         <v>1.69044506691566E-007</v>
@@ -5370,7 +5412,7 @@
         <v>9.06504201680673E-006</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
         <v>25</v>
       </c>
@@ -5435,7 +5477,8 @@
         <v>0</v>
       </c>
       <c r="V22" s="7" t="n">
-        <v>1.53676579520697E-005</v>
+        <f aca="false">SUM(E22:U22)</f>
+        <v>1.12010204137855E-008</v>
       </c>
       <c r="W22" s="7" t="n">
         <v>1.23699035169623E-007</v>
@@ -5444,7 +5487,7 @@
         <v>9.78428260192966E-006</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>25</v>
       </c>
@@ -5509,7 +5552,8 @@
         <v>2.39091987671193E-010</v>
       </c>
       <c r="V23" s="7" t="n">
-        <v>0.000217747864923747</v>
+        <f aca="false">SUM(E23:U23)</f>
+        <v>7.6033848401069E-008</v>
       </c>
       <c r="W23" s="7" t="n">
         <v>6.2977093059446E-006</v>
@@ -5518,7 +5562,7 @@
         <v>0.000148986725801432</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
         <v>25</v>
       </c>
@@ -5583,7 +5627,8 @@
         <v>0</v>
       </c>
       <c r="V24" s="7" t="n">
-        <v>9.87497721755369E-005</v>
+        <f aca="false">SUM(E24:U24)</f>
+        <v>3.52494016163066E-009</v>
       </c>
       <c r="W24" s="7" t="n">
         <v>3.16501400560224E-006</v>
@@ -5592,7 +5637,7 @@
         <v>7.05979707438531E-005</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>25</v>
       </c>
@@ -5657,7 +5702,8 @@
         <v>0</v>
       </c>
       <c r="V25" s="7" t="n">
-        <v>0.000278090569561158</v>
+        <f aca="false">SUM(E25:U25)</f>
+        <v>1.82706579029676E-007</v>
       </c>
       <c r="W25" s="7" t="n">
         <v>1.16542172424525E-005</v>
@@ -5666,7 +5712,7 @@
         <v>0.000174279489573607</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
         <v>25</v>
       </c>
@@ -5731,7 +5777,8 @@
         <v>0</v>
       </c>
       <c r="V26" s="7" t="n">
-        <v>0.00023080815437286</v>
+        <f aca="false">SUM(E26:U26)</f>
+        <v>1.21868726272532E-007</v>
       </c>
       <c r="W26" s="7" t="n">
         <v>4.06349206349206E-006</v>
@@ -5740,7 +5787,7 @@
         <v>0.000126291627762216</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
         <v>25</v>
       </c>
@@ -5805,7 +5852,8 @@
         <v>0</v>
       </c>
       <c r="V27" s="7" t="n">
-        <v>0.000212217736933259</v>
+        <f aca="false">SUM(E27:U27)</f>
+        <v>1.72263061897232E-007</v>
       </c>
       <c r="W27" s="7" t="n">
         <v>3.93907989090378E-005</v>
@@ -5814,7 +5862,7 @@
         <v>9.91723701863894E-005</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
         <v>25</v>
       </c>
@@ -5879,7 +5927,8 @@
         <v>1.92545819816825E-009</v>
       </c>
       <c r="V28" s="7" t="n">
-        <v>5.52998636530971E-005</v>
+        <f aca="false">SUM(E28:U28)</f>
+        <v>1.06355893352223E-008</v>
       </c>
       <c r="W28" s="7" t="n">
         <v>3.8129474011827E-006</v>
@@ -5888,7 +5937,7 @@
         <v>2.61501041658227E-005</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
         <v>25</v>
       </c>
@@ -5953,7 +6002,8 @@
         <v>0</v>
       </c>
       <c r="V29" s="7" t="n">
-        <v>0.000375226445804206</v>
+        <f aca="false">SUM(E29:U29)</f>
+        <v>2.41967408591707E-007</v>
       </c>
       <c r="W29" s="7" t="n">
         <v>1.40413649105153E-005</v>
@@ -5962,7 +6012,7 @@
         <v>0.000245013676384402</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
         <v>25</v>
       </c>
@@ -6027,7 +6077,8 @@
         <v>0</v>
       </c>
       <c r="V30" s="7" t="n">
-        <v>9.18631195351267E-006</v>
+        <f aca="false">SUM(E30:U30)</f>
+        <v>1.41728368796874E-009</v>
       </c>
       <c r="W30" s="7" t="n">
         <v>2.29192280303401E-007</v>
@@ -6036,7 +6087,7 @@
         <v>8.10233452503561E-006</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
         <v>25</v>
       </c>
@@ -6101,7 +6152,8 @@
         <v>0</v>
       </c>
       <c r="V31" s="7" t="n">
-        <v>0.000653934165917123</v>
+        <f aca="false">SUM(E31:U31)</f>
+        <v>5.0862219630936E-007</v>
       </c>
       <c r="W31" s="7" t="n">
         <v>1.88434112845717E-005</v>
@@ -6110,7 +6162,7 @@
         <v>0.000236656346812212</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
         <v>25</v>
       </c>
@@ -6175,7 +6227,8 @@
         <v>0</v>
       </c>
       <c r="V32" s="7" t="n">
-        <v>8.92975093926643E-005</v>
+        <f aca="false">SUM(E32:U32)</f>
+        <v>5.55636303707168E-008</v>
       </c>
       <c r="W32" s="7" t="n">
         <v>1.90469167040993E-005</v>
@@ -6184,7 +6237,7 @@
         <v>0.000232956214937649</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
         <v>25</v>
       </c>
@@ -6249,7 +6302,8 @@
         <v>0</v>
       </c>
       <c r="V33" s="7" t="n">
-        <v>0.000116323614167505</v>
+        <f aca="false">SUM(E33:U33)</f>
+        <v>9.11331208528063E-008</v>
       </c>
       <c r="W33" s="7" t="n">
         <v>1.45273690731029E-006</v>
@@ -6258,7 +6312,7 @@
         <v>7.34224184754248E-005</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
         <v>25</v>
       </c>
@@ -6323,7 +6377,8 @@
         <v>0</v>
       </c>
       <c r="V34" s="7" t="n">
-        <v>0.000135206740639641</v>
+        <f aca="false">SUM(E34:U34)</f>
+        <v>1.29474954432514E-007</v>
       </c>
       <c r="W34" s="7" t="n">
         <v>1.12703856571946E-005</v>
@@ -6332,7 +6387,7 @@
         <v>7.54697313675911E-005</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
         <v>25</v>
       </c>
@@ -6397,7 +6452,8 @@
         <v>0</v>
       </c>
       <c r="V35" s="7" t="n">
-        <v>3.47272112205559E-005</v>
+        <f aca="false">SUM(E35:U35)</f>
+        <v>1.05095052842381E-008</v>
       </c>
       <c r="W35" s="7" t="n">
         <v>4.52483832131708E-006</v>
@@ -6406,7 +6462,7 @@
         <v>1.18843356980872E-005</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
         <v>25</v>
       </c>
@@ -6471,7 +6527,8 @@
         <v>0</v>
       </c>
       <c r="V36" s="7" t="n">
-        <v>0.000137535942229496</v>
+        <f aca="false">SUM(E36:U36)</f>
+        <v>5.03350679926345E-008</v>
       </c>
       <c r="W36" s="7" t="n">
         <v>3.92155062051743E-006</v>
@@ -6480,7 +6537,7 @@
         <v>8.66117227497538E-005</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
         <v>25</v>
       </c>
@@ -6545,7 +6602,8 @@
         <v>0</v>
       </c>
       <c r="V37" s="7" t="n">
-        <v>8.05839229213638E-005</v>
+        <f aca="false">SUM(E37:U37)</f>
+        <v>2.14026567151602E-008</v>
       </c>
       <c r="W37" s="7" t="n">
         <v>7.8706485511225E-006</v>
@@ -6554,7 +6612,7 @@
         <v>4.7295504808849E-005</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
         <v>25</v>
       </c>
@@ -6619,7 +6677,8 @@
         <v>0</v>
       </c>
       <c r="V38" s="7" t="n">
-        <v>1.41412300914954E-005</v>
+        <f aca="false">SUM(E38:U38)</f>
+        <v>3.91960092113541E-009</v>
       </c>
       <c r="W38" s="7" t="n">
         <v>4.28945613741018E-006</v>
@@ -6628,7 +6687,7 @@
         <v>6.50721411787057E-006</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
         <v>25</v>
       </c>
@@ -6693,7 +6752,8 @@
         <v>0</v>
       </c>
       <c r="V39" s="7" t="n">
-        <v>4.94175933965979E-005</v>
+        <f aca="false">SUM(E39:U39)</f>
+        <v>9.08497078414461E-009</v>
       </c>
       <c r="W39" s="7" t="n">
         <v>8.68402518706015E-006</v>
@@ -6702,7 +6762,7 @@
         <v>1.87623456906989E-005</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
         <v>25</v>
       </c>
@@ -6767,7 +6827,8 @@
         <v>0</v>
       </c>
       <c r="V40" s="7" t="n">
-        <v>4.19921400756668E-005</v>
+        <f aca="false">SUM(E40:U40)</f>
+        <v>7.61860068531485E-009</v>
       </c>
       <c r="W40" s="7" t="n">
         <v>4.68132945468852E-006</v>
@@ -6776,7 +6837,7 @@
         <v>3.11999877138856E-005</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
         <v>25</v>
       </c>
@@ -6841,7 +6902,8 @@
         <v>0</v>
       </c>
       <c r="V41" s="7" t="n">
-        <v>1.55419079500978E-005</v>
+        <f aca="false">SUM(E41:U41)</f>
+        <v>4.13200437503889E-009</v>
       </c>
       <c r="W41" s="7" t="n">
         <v>2.32584810200019E-006</v>
@@ -6850,7 +6912,7 @@
         <v>8.34805599261492E-006</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
         <v>25</v>
       </c>
@@ -6915,7 +6977,8 @@
         <v>2.45619281875655E-008</v>
       </c>
       <c r="V42" s="7" t="n">
-        <v>0.000177043967890465</v>
+        <f aca="false">SUM(E42:U42)</f>
+        <v>3.07571148344275E-007</v>
       </c>
       <c r="W42" s="7" t="n">
         <v>8.65941910229048E-006</v>
@@ -6924,7 +6987,7 @@
         <v>0.000109230271128868</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
         <v>25</v>
       </c>
@@ -6989,7 +7052,8 @@
         <v>2.96949419218293E-010</v>
       </c>
       <c r="V43" s="7" t="n">
-        <v>9.6531557362526E-005</v>
+        <f aca="false">SUM(E43:U43)</f>
+        <v>3.11245263273904E-008</v>
       </c>
       <c r="W43" s="7" t="n">
         <v>6.82604727805026E-006</v>
@@ -8168,10 +8232,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8219,6 +8283,9 @@
       <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="N1" s="23" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -8260,6 +8327,9 @@
       <c r="M2" s="0" t="n">
         <v>5.48488227400302</v>
       </c>
+      <c r="N2" s="0" t="n">
+        <v>7.3482069736456</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -8301,6 +8371,9 @@
       <c r="M3" s="0" t="n">
         <v>2.60926606216575</v>
       </c>
+      <c r="N3" s="0" t="n">
+        <v>3.67555245089079</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -8342,6 +8415,9 @@
       <c r="M4" s="0" t="n">
         <v>6.22549391704</v>
       </c>
+      <c r="N4" s="0" t="n">
+        <v>7.7494</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -8383,6 +8459,9 @@
       <c r="M5" s="0" t="n">
         <v>1.74677976836</v>
       </c>
+      <c r="N5" s="0" t="n">
+        <v>2.7947</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -8394,7 +8473,7 @@
       <c r="C6" s="0" t="n">
         <v>69.4866667310927</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="24" t="n">
         <v>3.55495857846617</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -8423,6 +8502,9 @@
       </c>
       <c r="M6" s="0" t="n">
         <v>3.24065352308549</v>
+      </c>
+      <c r="N6" s="25" t="n">
+        <v>115.962814684184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8465,6 +8547,9 @@
       <c r="M7" s="0" t="n">
         <v>4.56076901820934</v>
       </c>
+      <c r="N7" s="25" t="n">
+        <v>168.193913397624</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -8506,6 +8591,9 @@
       <c r="M8" s="0" t="n">
         <v>4.70419091891999</v>
       </c>
+      <c r="N8" s="25" t="n">
+        <v>70.2568127278382</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -8547,6 +8635,9 @@
       <c r="M9" s="0" t="n">
         <v>14.3126164539504</v>
       </c>
+      <c r="N9" s="25" t="n">
+        <v>125.389167088083</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -8558,35 +8649,38 @@
       <c r="C10" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="24" t="s">
+      <c r="L10" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="26" t="s">
         <v>63</v>
+      </c>
+      <c r="N10" s="26" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8596,38 +8690,41 @@
       <c r="B11" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="E11" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="G11" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="I11" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="K11" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="26" t="s">
         <v>74</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="N11" s="26" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subo figuras modificadas para OG
</commit_message>
<xml_diff>
--- a/sedDegr.xlsx
+++ b/sedDegr.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WFL" sheetId="1" state="visible" r:id="rId2"/>
@@ -99,6 +99,9 @@
     <t>N</t>
   </si>
   <si>
+    <t>Sitosterol</t>
+  </si>
+  <si>
     <t>Media Sed BZ</t>
   </si>
   <si>
@@ -166,21 +169,6 @@
   </si>
   <si>
     <t>site</t>
-  </si>
-  <si>
-    <r>
-      <t>β</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>-Sitosterol</t>
-    </r>
   </si>
   <si>
     <t>Acc Eff</t>
@@ -290,7 +278,7 @@
     <numFmt numFmtId="171" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="172" formatCode="0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -334,13 +322,6 @@
     <font>
       <sz val="9"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -430,7 +411,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -519,11 +500,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,7 +512,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3828,8 +3805,8 @@
   </sheetPr>
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3867,7 +3844,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
@@ -7091,7 +7068,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="14"/>
       <c r="Y1" s="14"/>
@@ -7099,7 +7076,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="15"/>
       <c r="Y2" s="15"/>
@@ -7107,7 +7084,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">100-67.87</f>
@@ -7116,7 +7093,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2.65</v>
@@ -7124,7 +7101,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="16" t="n">
         <f aca="false">WFL!D44</f>
@@ -7133,7 +7110,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="17" t="n">
         <f aca="false">Sheet3!B5/Sheet3!B4</f>
@@ -7142,7 +7119,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="18" t="n">
         <f aca="false">WFL!D46</f>
@@ -7151,7 +7128,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="19" t="n">
         <f aca="false">Sheet3!B7/Sheet3!B4</f>
@@ -7160,18 +7137,18 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>12.52</v>
@@ -7179,13 +7156,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>4.73</v>
@@ -7193,18 +7170,18 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>0.55</v>
@@ -7212,13 +7189,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>0.21</v>
@@ -7226,16 +7203,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7571,7 +7548,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>20</v>
@@ -7623,16 +7600,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7981,7 +7958,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8234,8 +8211,8 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8245,10 +8222,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -8262,8 +8239,8 @@
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>49</v>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>11</v>
@@ -8283,7 +8260,7 @@
       <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="22" t="s">
         <v>21</v>
       </c>
     </row>
@@ -8473,7 +8450,7 @@
       <c r="C6" s="0" t="n">
         <v>69.4866667310927</v>
       </c>
-      <c r="D6" s="24" t="n">
+      <c r="D6" s="23" t="n">
         <v>3.55495857846617</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -8503,7 +8480,7 @@
       <c r="M6" s="0" t="n">
         <v>3.24065352308549</v>
       </c>
-      <c r="N6" s="25" t="n">
+      <c r="N6" s="24" t="n">
         <v>115.962814684184</v>
       </c>
     </row>
@@ -8547,7 +8524,7 @@
       <c r="M7" s="0" t="n">
         <v>4.56076901820934</v>
       </c>
-      <c r="N7" s="25" t="n">
+      <c r="N7" s="24" t="n">
         <v>168.193913397624</v>
       </c>
     </row>
@@ -8591,7 +8568,7 @@
       <c r="M8" s="0" t="n">
         <v>4.70419091891999</v>
       </c>
-      <c r="N8" s="25" t="n">
+      <c r="N8" s="24" t="n">
         <v>70.2568127278382</v>
       </c>
     </row>
@@ -8635,7 +8612,7 @@
       <c r="M9" s="0" t="n">
         <v>14.3126164539504</v>
       </c>
-      <c r="N9" s="25" t="n">
+      <c r="N9" s="24" t="n">
         <v>125.389167088083</v>
       </c>
     </row>
@@ -8649,37 +8626,37 @@
       <c r="C10" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="26" t="s">
+      <c r="L10" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="26" t="s">
+      <c r="M10" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="N10" s="25" t="s">
         <v>64</v>
       </c>
     </row>
@@ -8690,40 +8667,40 @@
       <c r="B11" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="26" t="s">
+      <c r="L11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="M11" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="N11" s="26" t="s">
+      <c r="N11" s="25" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>